<commit_message>
Speedup calc added to script; Speedup Graph added
</commit_message>
<xml_diff>
--- a/Scripts/Cluster Graphs.xlsx
+++ b/Scripts/Cluster Graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\8º Semestre\CP\Works\CP_Entrega\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C65715-0765-4522-97DE-42BB8BFBFEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AC83AB-86DA-4C24-A6DB-E23D0B1F120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-1605" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Threads</t>
   </si>
@@ -33,19 +33,20 @@
     <t>Testes</t>
   </si>
   <si>
-    <t>melhora</t>
+    <t>SpeedUp</t>
   </si>
   <si>
-    <t>piora</t>
-  </si>
-  <si>
-    <t>constante</t>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,7 +64,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -71,13 +72,281 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,24 +475,24 @@
             <c:numRef>
               <c:f>Plan1!$C$3:$H$3</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>28.170249999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>19.636672669999999</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>18.027305999999999</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>16.999802330000001</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>17.04534533</c:v>
                 </c:pt>
               </c:numCache>
@@ -256,6 +525,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -322,7 +646,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -596,6 +980,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -663,6 +1102,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -884,7 +1378,7 @@
             <c:numRef>
               <c:f>Plan1!$C$5:$H$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>4.41</c:v>
@@ -934,6 +1428,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1001,7 +1550,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1222,7 +1826,7 @@
             <c:numRef>
               <c:f>Plan1!$C$6:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>152</c:v>
@@ -1272,6 +1876,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1339,7 +1998,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1383,6 +2097,738 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SpeedUp</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$O$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$O$3:$S$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.2788183841153999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.43457348799316</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5626433589134101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.65709279717703</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6526652554765799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E8CF-4F0D-860E-672EE7AC97CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Test 9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$O$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$O$4:$S$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.14055793991416299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5157773952954601E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9624924379915299E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7282043665527906E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.02295798844291E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E8CF-4F0D-860E-672EE7AC97CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test 10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$O$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$O$5:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0116775549457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98770269985624304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.01147349013831</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99990222734131795</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99973803044864895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E8CF-4F0D-860E-672EE7AC97CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Test 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$O$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$O$6:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.99449819573824105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99731066662615897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99481319866683804</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99473148904130204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99427229161071895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E8CF-4F0D-860E-672EE7AC97CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="385828544"/>
+        <c:axId val="385843936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="385828544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385843936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="385843936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.7000000000000002"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t>Speed Up </a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385828544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1587,6 +3033,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3097,6 +4583,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3751,6 +5740,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C10B38E-D3DE-4B83-B1B6-F351FF864760}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4017,160 +6044,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="25"/>
+      <c r="N1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C2">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="11">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="12">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="12">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="12">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="12">
         <v>16</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="13">
         <v>32</v>
       </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="11">
+        <v>1</v>
+      </c>
+      <c r="O2" s="12">
+        <v>2</v>
+      </c>
+      <c r="P2" s="12">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>8</v>
+      </c>
+      <c r="R2" s="12">
+        <v>16</v>
+      </c>
+      <c r="S2" s="13">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="23">
         <v>28.170249999999999</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="24">
         <v>22</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="24">
         <v>19.636672669999999</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="24">
         <v>18.027305999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="24">
         <v>16.999802330000001</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="24">
         <v>17.04534533</v>
       </c>
-      <c r="I3">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>8</v>
+      </c>
+      <c r="N3" s="16">
+        <v>1</v>
+      </c>
+      <c r="O3" s="17">
+        <v>1.2788183841153999</v>
+      </c>
+      <c r="P3" s="17">
+        <v>1.43457348799316</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>1.5626433589134101</v>
+      </c>
+      <c r="R3" s="17">
+        <v>1.65709279717703</v>
+      </c>
+      <c r="S3" s="17">
+        <v>1.6526652554765799</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9">
+        <v>9</v>
+      </c>
+      <c r="C4" s="15">
+        <v>4.3699999999999998E-5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3.1100000000000002E-4</v>
+      </c>
+      <c r="E4" s="14">
+        <v>5.8100000000000003E-4</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G4" s="14">
+        <v>4.4900000000000001E-3</v>
+      </c>
+      <c r="H4" s="14">
+        <v>4.2700000000000004E-3</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="9">
+        <v>9</v>
+      </c>
+      <c r="N4" s="16">
+        <v>1</v>
+      </c>
+      <c r="O4" s="18">
+        <v>0.14055793991416299</v>
+      </c>
+      <c r="P4" s="18">
+        <v>7.5157773952954601E-2</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>3.9624924379915299E-2</v>
+      </c>
+      <c r="R4" s="18">
+        <v>9.7282043665527906E-3</v>
+      </c>
+      <c r="S4" s="18">
+        <v>1.02295798844291E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="9">
+        <v>10</v>
+      </c>
+      <c r="C5" s="21">
+        <v>4.41</v>
+      </c>
+      <c r="D5" s="22">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E5" s="22">
+        <v>4.46</v>
+      </c>
+      <c r="F5" s="22">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="G5" s="22">
+        <v>4.41</v>
+      </c>
+      <c r="H5" s="22">
+        <v>4.41</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="9">
+        <v>10</v>
+      </c>
+      <c r="N5" s="16">
+        <v>1</v>
+      </c>
+      <c r="O5" s="18">
+        <v>1.0116775549457</v>
+      </c>
+      <c r="P5" s="18">
+        <v>0.98770269985624304</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>1.01147349013831</v>
+      </c>
+      <c r="R5" s="18">
+        <v>0.99990222734131795</v>
+      </c>
+      <c r="S5" s="18">
+        <v>0.99973803044864895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4.3699999999999998E-5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3.1100000000000002E-4</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.8100000000000003E-4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>4.4900000000000001E-3</v>
-      </c>
-      <c r="H4" s="1">
-        <v>4.2700000000000004E-3</v>
-      </c>
-      <c r="I4">
+      <c r="C6" s="19">
+        <v>152</v>
+      </c>
+      <c r="D6" s="20">
+        <v>152</v>
+      </c>
+      <c r="E6" s="20">
+        <v>152</v>
+      </c>
+      <c r="F6" s="20">
+        <v>152</v>
+      </c>
+      <c r="G6" s="20">
+        <v>152</v>
+      </c>
+      <c r="H6" s="20">
+        <v>153</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="10">
+        <v>2</v>
+      </c>
+      <c r="N6" s="16">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4.41</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4.46</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="G5" s="1">
-        <v>4.41</v>
-      </c>
-      <c r="H5" s="1">
-        <v>4.41</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>152</v>
-      </c>
-      <c r="D6" s="1">
-        <v>152</v>
-      </c>
-      <c r="E6" s="1">
-        <v>152</v>
-      </c>
-      <c r="F6" s="1">
-        <v>152</v>
-      </c>
-      <c r="G6" s="1">
-        <v>152</v>
-      </c>
-      <c r="H6" s="1">
-        <v>153</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
+      <c r="O6" s="18">
+        <v>0.99449819573824105</v>
+      </c>
+      <c r="P6" s="18">
+        <v>0.99731066662615897</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>0.99481319866683804</v>
+      </c>
+      <c r="R6" s="18">
+        <v>0.99473148904130204</v>
+      </c>
+      <c r="S6" s="18">
+        <v>0.99427229161071895</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L3:L6"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Efficiency and Cost graphs added
</commit_message>
<xml_diff>
--- a/Scripts/Cluster Graphs.xlsx
+++ b/Scripts/Cluster Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\8º Semestre\CP\Works\CP_Entrega\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BE722-C614-4CCA-B123-FC3E72B67FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8670178B-52AC-4A9C-BECD-4B551CA30120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-1605" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -342,6 +342,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,7 +373,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2900,6 +2903,1509 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Efficiency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AC$3:$AG$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AC$4:$AG$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.64023295454545504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35864337193741003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19533041986417798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10356829984387299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1645789243743002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C5BF-4006-9DDE-5538D7DCB47B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Test 9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AC$3:$AG$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AC$5:$AG$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.0257234726688003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8803786574871001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9659090909089992E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0829621380799987E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1981850117100002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C5BF-4006-9DDE-5538D7DCB47B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test 10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AC$3:$AG$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AC$6:$AG$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.50573394495413004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24719730941704099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12643348623853301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.125E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C5BF-4006-9DDE-5538D7DCB47B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Test 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AC$3:$AG$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AC$7:$AG$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1045751633986998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C5BF-4006-9DDE-5538D7DCB47B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="385828544"/>
+        <c:axId val="385843936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="385828544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385843936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="385843936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385828544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cost</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AI$3:$AM$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AI$4:$AM$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.546690679999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144.218448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>271.99683728000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>545.45105056</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C973-40D2-83BF-4D342C8520A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Test 9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AI$3:$AM$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AI$5:$AM$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.2200000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3239999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8000000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1840000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13664000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C973-40D2-83BF-4D342C8520A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test 10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AI$3:$AM$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AI$6:$AM$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.7200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>141.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C973-40D2-83BF-4D342C8520A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Test 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$AI$3:$AM$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$AI$7:$AM$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1216</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2432</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C973-40D2-83BF-4D342C8520A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="385828544"/>
+        <c:axId val="385843936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="385828544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385843936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="385843936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" baseline="0"/>
+                  <a:t>Cost</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="385828544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="250"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3100,6 +4606,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5113,6 +6699,1012 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5805,6 +8397,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>24653</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E0D427-AB72-4529-B70A-EED72DD12D49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>24652</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39216CB6-B016-4DEB-8E33-9BFBA2674AFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6073,41 +8741,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:AM7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
-      <c r="L1" s="24" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="L1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="21" t="s">
+      <c r="M1" s="26"/>
+      <c r="N1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="4">
         <v>1</v>
       </c>
@@ -6126,8 +8794,8 @@
       <c r="H2" s="6">
         <v>32</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
       <c r="N2" s="4">
         <v>1</v>
       </c>
@@ -6146,39 +8814,39 @@
       <c r="S2" s="6">
         <v>32</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28" t="s">
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" s="28" t="s">
+      <c r="AD2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28" t="s">
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -6202,7 +8870,7 @@
       <c r="H3" s="17">
         <v>17.04534533</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="M3" s="1">
@@ -6226,57 +8894,57 @@
       <c r="S3" s="10">
         <v>1.6526652554765799</v>
       </c>
-      <c r="V3" s="28">
+      <c r="V3" s="18">
         <v>2</v>
       </c>
-      <c r="W3" s="28">
+      <c r="W3" s="18">
         <v>4</v>
       </c>
-      <c r="X3" s="28">
+      <c r="X3" s="18">
         <v>8</v>
       </c>
-      <c r="Y3" s="28">
+      <c r="Y3" s="18">
         <v>16</v>
       </c>
-      <c r="Z3" s="28">
+      <c r="Z3" s="18">
         <v>32</v>
       </c>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28">
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18">
         <v>2</v>
       </c>
-      <c r="AD3" s="28">
+      <c r="AD3" s="18">
         <v>4</v>
       </c>
-      <c r="AE3" s="28">
+      <c r="AE3" s="18">
         <v>8</v>
       </c>
-      <c r="AF3" s="28">
+      <c r="AF3" s="18">
         <v>16</v>
       </c>
-      <c r="AG3" s="28">
+      <c r="AG3" s="18">
         <v>32</v>
       </c>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="28">
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18">
         <v>2</v>
       </c>
-      <c r="AJ3" s="28">
+      <c r="AJ3" s="18">
         <v>4</v>
       </c>
-      <c r="AK3" s="28">
+      <c r="AK3" s="18">
         <v>8</v>
       </c>
-      <c r="AL3" s="28">
+      <c r="AL3" s="18">
         <v>16</v>
       </c>
-      <c r="AM3" s="28">
+      <c r="AM3" s="18">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2">
         <v>9</v>
       </c>
@@ -6298,7 +8966,7 @@
       <c r="H4" s="7">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="L4" s="19"/>
+      <c r="L4" s="20"/>
       <c r="M4" s="2">
         <v>9</v>
       </c>
@@ -6320,57 +8988,57 @@
       <c r="S4" s="11">
         <v>1.02295798844291E-2</v>
       </c>
-      <c r="V4" s="28">
+      <c r="V4" s="18">
         <v>1.2804659090909101</v>
       </c>
-      <c r="W4" s="28">
+      <c r="W4" s="18">
         <v>1.4345734877496401</v>
       </c>
-      <c r="X4" s="28">
+      <c r="X4" s="18">
         <v>1.5626433589134201</v>
       </c>
-      <c r="Y4" s="28">
+      <c r="Y4" s="18">
         <v>1.65709279750196</v>
       </c>
-      <c r="Z4" s="28">
+      <c r="Z4" s="18">
         <v>1.6526652557997801</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28">
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18">
         <v>0.64023295454545504</v>
       </c>
-      <c r="AD4" s="28">
+      <c r="AD4" s="18">
         <v>0.35864337193741003</v>
       </c>
-      <c r="AE4" s="28">
+      <c r="AE4" s="18">
         <v>0.19533041986417798</v>
       </c>
-      <c r="AF4" s="28">
+      <c r="AF4" s="18">
         <v>0.10356829984387299</v>
       </c>
-      <c r="AG4" s="28">
+      <c r="AG4" s="18">
         <v>5.1645789243743002E-2</v>
       </c>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="28">
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="29">
         <v>44</v>
       </c>
-      <c r="AJ4" s="28">
+      <c r="AJ4" s="29">
         <v>78.546690679999998</v>
       </c>
-      <c r="AK4" s="28">
+      <c r="AK4" s="29">
         <v>144.218448</v>
       </c>
-      <c r="AL4" s="28">
+      <c r="AL4" s="29">
         <v>271.99683728000002</v>
       </c>
-      <c r="AM4" s="28">
+      <c r="AM4" s="29">
         <v>545.45105056</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -6392,7 +9060,7 @@
       <c r="H5" s="15">
         <v>4.41</v>
       </c>
-      <c r="L5" s="19"/>
+      <c r="L5" s="20"/>
       <c r="M5" s="2">
         <v>10</v>
       </c>
@@ -6414,57 +9082,57 @@
       <c r="S5" s="11">
         <v>0.99973803044864895</v>
       </c>
-      <c r="V5" s="28">
+      <c r="V5" s="18">
         <v>0.14051446945337601</v>
       </c>
-      <c r="W5" s="28">
+      <c r="W5" s="18">
         <v>7.5215146299484004E-2</v>
       </c>
-      <c r="X5" s="28">
+      <c r="X5" s="18">
         <v>3.9727272727273E-2</v>
       </c>
-      <c r="Y5" s="28">
+      <c r="Y5" s="18">
         <v>9.7327394209349993E-3</v>
       </c>
-      <c r="Z5" s="28">
+      <c r="Z5" s="18">
         <v>1.0234192037471E-2</v>
       </c>
-      <c r="AA5" s="28"/>
-      <c r="AB5" s="28"/>
-      <c r="AC5" s="28">
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18">
         <v>7.0257234726688003E-2</v>
       </c>
-      <c r="AD5" s="28">
+      <c r="AD5" s="18">
         <v>1.8803786574871001E-2</v>
       </c>
-      <c r="AE5" s="28">
+      <c r="AE5" s="18">
         <v>4.9659090909089992E-3</v>
       </c>
-      <c r="AF5" s="28">
+      <c r="AF5" s="18">
         <v>6.0829621380799987E-4</v>
       </c>
-      <c r="AG5" s="28">
+      <c r="AG5" s="18">
         <v>3.1981850117100002E-4</v>
       </c>
-      <c r="AH5" s="28"/>
-      <c r="AI5" s="28">
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="29">
         <v>6.2200000000000005E-4</v>
       </c>
-      <c r="AJ5" s="28">
+      <c r="AJ5" s="29">
         <v>2.3239999999999997E-3</v>
       </c>
-      <c r="AK5" s="28">
+      <c r="AK5" s="29">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="AL5" s="28">
+      <c r="AL5" s="29">
         <v>7.1840000000000001E-2</v>
       </c>
-      <c r="AM5" s="28">
+      <c r="AM5" s="29">
         <v>0.13664000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -6486,7 +9154,7 @@
       <c r="H6" s="13">
         <v>153</v>
       </c>
-      <c r="L6" s="20"/>
+      <c r="L6" s="21"/>
       <c r="M6" s="3">
         <v>2</v>
       </c>
@@ -6508,102 +9176,102 @@
       <c r="S6" s="11">
         <v>0.99427229161071895</v>
       </c>
-      <c r="V6" s="28">
+      <c r="V6" s="18">
         <v>1.0114678899082601</v>
       </c>
-      <c r="W6" s="28">
+      <c r="W6" s="18">
         <v>0.98878923766816196</v>
       </c>
-      <c r="X6" s="28">
+      <c r="X6" s="18">
         <v>1.0114678899082601</v>
       </c>
-      <c r="Y6" s="28">
+      <c r="Y6" s="18">
         <v>1</v>
       </c>
-      <c r="Z6" s="28">
+      <c r="Z6" s="18">
         <v>1</v>
       </c>
-      <c r="AA6" s="28"/>
-      <c r="AB6" s="28"/>
-      <c r="AC6" s="28">
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18">
         <v>0.50573394495413004</v>
       </c>
-      <c r="AD6" s="28">
+      <c r="AD6" s="18">
         <v>0.24719730941704099</v>
       </c>
-      <c r="AE6" s="28">
+      <c r="AE6" s="18">
         <v>0.12643348623853301</v>
       </c>
-      <c r="AF6" s="28">
+      <c r="AF6" s="18">
         <v>6.25E-2</v>
       </c>
-      <c r="AG6" s="28">
+      <c r="AG6" s="18">
         <v>3.125E-2</v>
       </c>
-      <c r="AH6" s="28"/>
-      <c r="AI6" s="28">
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="29">
         <v>8.7200000000000006</v>
       </c>
-      <c r="AJ6" s="28">
+      <c r="AJ6" s="29">
         <v>17.84</v>
       </c>
-      <c r="AK6" s="28">
+      <c r="AK6" s="29">
         <v>34.880000000000003</v>
       </c>
-      <c r="AL6" s="28">
+      <c r="AL6" s="29">
         <v>70.56</v>
       </c>
-      <c r="AM6" s="28">
+      <c r="AM6" s="29">
         <v>141.12</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="V7" s="28">
+      <c r="V7" s="18">
         <v>1</v>
       </c>
-      <c r="W7" s="28">
+      <c r="W7" s="18">
         <v>1</v>
       </c>
-      <c r="X7" s="28">
+      <c r="X7" s="18">
         <v>1</v>
       </c>
-      <c r="Y7" s="28">
+      <c r="Y7" s="18">
         <v>1</v>
       </c>
-      <c r="Z7" s="28">
+      <c r="Z7" s="18">
         <v>0.99346405228758194</v>
       </c>
-      <c r="AA7" s="28"/>
-      <c r="AB7" s="28"/>
-      <c r="AC7" s="28">
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18">
         <v>0.5</v>
       </c>
-      <c r="AD7" s="28">
+      <c r="AD7" s="18">
         <v>0.25</v>
       </c>
-      <c r="AE7" s="28">
+      <c r="AE7" s="18">
         <v>0.125</v>
       </c>
-      <c r="AF7" s="28">
+      <c r="AF7" s="18">
         <v>6.25E-2</v>
       </c>
-      <c r="AG7" s="28">
+      <c r="AG7" s="18">
         <v>3.1045751633986998E-2</v>
       </c>
-      <c r="AH7" s="28"/>
-      <c r="AI7" s="28">
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="29">
         <v>304</v>
       </c>
-      <c r="AJ7" s="28">
+      <c r="AJ7" s="29">
         <v>608</v>
       </c>
-      <c r="AK7" s="28">
+      <c r="AK7" s="29">
         <v>1216</v>
       </c>
-      <c r="AL7" s="28">
+      <c r="AL7" s="29">
         <v>2432</v>
       </c>
-      <c r="AM7" s="28">
+      <c r="AM7" s="29">
         <v>4896</v>
       </c>
     </row>

</xml_diff>